<commit_message>
Going to the Sky!
</commit_message>
<xml_diff>
--- a/just-random/class-control.xlsx
+++ b/just-random/class-control.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFE90D9-5D65-439C-816F-EE5A09C381C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10545" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new-GoStack" sheetId="1" state="hidden" r:id="rId1"/>
@@ -1553,7 +1554,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -2082,7 +2083,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2120,9 +2121,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2155,9 +2156,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2190,9 +2208,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2365,7 +2400,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -6296,14 +6331,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF66FF"/>
   </sheetPr>
   <dimension ref="C3:R303"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J111" sqref="J111"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B112" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J115" sqref="J115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8310,13 +8345,13 @@
     </row>
     <row r="111" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C111" s="34"/>
-      <c r="D111" s="13" t="s">
+      <c r="D111" s="52" t="s">
         <v>390</v>
       </c>
-      <c r="E111" s="13">
+      <c r="E111" s="52">
         <v>3</v>
       </c>
-      <c r="F111" s="19">
+      <c r="F111" s="53">
         <v>56</v>
       </c>
       <c r="G111" s="35"/>
@@ -8327,13 +8362,13 @@
     </row>
     <row r="112" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C112" s="34"/>
-      <c r="D112" s="13" t="s">
+      <c r="D112" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="E112" s="13">
+      <c r="E112" s="52">
         <v>4</v>
       </c>
-      <c r="F112" s="19">
+      <c r="F112" s="53">
         <v>23</v>
       </c>
       <c r="G112" s="35"/>
@@ -8344,13 +8379,13 @@
     </row>
     <row r="113" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C113" s="34"/>
-      <c r="D113" s="13" t="s">
+      <c r="D113" s="52" t="s">
         <v>206</v>
       </c>
-      <c r="E113" s="13">
+      <c r="E113" s="52">
         <v>5</v>
       </c>
-      <c r="F113" s="19">
+      <c r="F113" s="53">
         <v>31</v>
       </c>
       <c r="G113" s="35"/>
@@ -8361,13 +8396,13 @@
     </row>
     <row r="114" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C114" s="34"/>
-      <c r="D114" s="13" t="s">
+      <c r="D114" s="52" t="s">
         <v>391</v>
       </c>
-      <c r="E114" s="13">
+      <c r="E114" s="52">
         <v>9</v>
       </c>
-      <c r="F114" s="19">
+      <c r="F114" s="53">
         <v>31</v>
       </c>
       <c r="G114" s="35"/>
@@ -8378,13 +8413,13 @@
     </row>
     <row r="115" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C115" s="34"/>
-      <c r="D115" s="13" t="s">
+      <c r="D115" s="52" t="s">
         <v>392</v>
       </c>
-      <c r="E115" s="13">
+      <c r="E115" s="52">
         <v>10</v>
       </c>
-      <c r="F115" s="19">
+      <c r="F115" s="53">
         <v>47</v>
       </c>
       <c r="G115" s="35"/>
@@ -8395,13 +8430,13 @@
     </row>
     <row r="116" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C116" s="34"/>
-      <c r="D116" s="13" t="s">
+      <c r="D116" s="52" t="s">
         <v>393</v>
       </c>
-      <c r="E116" s="13">
+      <c r="E116" s="52">
         <v>3</v>
       </c>
-      <c r="F116" s="19">
+      <c r="F116" s="53">
         <v>36</v>
       </c>
       <c r="G116" s="35"/>
@@ -8412,13 +8447,13 @@
     </row>
     <row r="117" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C117" s="34"/>
-      <c r="D117" s="13" t="s">
+      <c r="D117" s="52" t="s">
         <v>394</v>
       </c>
-      <c r="E117" s="13">
+      <c r="E117" s="52">
         <v>5</v>
       </c>
-      <c r="F117" s="19">
+      <c r="F117" s="53">
         <v>57</v>
       </c>
       <c r="G117" s="35"/>

</xml_diff>

<commit_message>
Nobody cant stop me!
</commit_message>
<xml_diff>
--- a/just-random/class-control.xlsx
+++ b/just-random/class-control.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D4D96D-75F9-4E9D-A7CB-86E260FEE795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10545" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="new-GoStack" sheetId="1" state="hidden" r:id="rId1"/>
@@ -1554,7 +1553,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -2083,7 +2082,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2121,9 +2120,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2156,26 +2155,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2208,26 +2190,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2400,7 +2365,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -6331,14 +6296,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF66FF"/>
   </sheetPr>
   <dimension ref="C3:R303"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B124" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M141" sqref="M141"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B169" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H146" sqref="H146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8719,13 +8684,13 @@
     </row>
     <row r="133" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C133" s="34"/>
-      <c r="D133" s="13" t="s">
+      <c r="D133" s="52" t="s">
         <v>410</v>
       </c>
-      <c r="E133" s="13">
+      <c r="E133" s="52">
         <v>6</v>
       </c>
-      <c r="F133" s="19">
+      <c r="F133" s="53">
         <v>20</v>
       </c>
       <c r="G133" s="24" t="s">
@@ -8744,28 +8709,28 @@
     </row>
     <row r="134" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C134" s="34"/>
-      <c r="D134" s="14" t="s">
+      <c r="D134" s="54" t="s">
         <v>411</v>
       </c>
-      <c r="E134" s="14">
+      <c r="E134" s="54">
         <v>4</v>
       </c>
-      <c r="F134" s="20">
+      <c r="F134" s="55">
         <v>59</v>
       </c>
-      <c r="G134" s="7">
+      <c r="G134" s="57">
         <f>SUM(E109:E134)</f>
         <v>142</v>
       </c>
-      <c r="H134" s="2">
+      <c r="H134" s="58">
         <f>SUM(F109:F134)</f>
         <v>785</v>
       </c>
-      <c r="I134" s="6">
+      <c r="I134" s="59">
         <f>G134+(H134/60)</f>
         <v>155.08333333333334</v>
       </c>
-      <c r="J134" s="5" t="s">
+      <c r="J134" s="56" t="s">
         <v>296</v>
       </c>
       <c r="K134" s="37"/>

</xml_diff>

<commit_message>
mod07 n' 08 finalized!
</commit_message>
<xml_diff>
--- a/just-random/class-control.xlsx
+++ b/just-random/class-control.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35440D43-8FAA-4391-8A5C-B61DDA87CCC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10545" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new-GoStack" sheetId="1" state="hidden" r:id="rId1"/>
@@ -1553,7 +1554,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -2082,7 +2083,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2120,9 +2121,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2155,9 +2156,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2190,9 +2208,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2365,7 +2400,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -6296,14 +6331,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF66FF"/>
   </sheetPr>
   <dimension ref="C3:R303"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B169" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H146" sqref="H146"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B133" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N149" sqref="N149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8737,13 +8772,13 @@
     </row>
     <row r="135" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C135" s="34"/>
-      <c r="D135" s="9" t="s">
+      <c r="D135" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="E135" s="9">
+      <c r="E135" s="44">
         <v>1</v>
       </c>
-      <c r="F135" s="15">
+      <c r="F135" s="45">
         <v>49</v>
       </c>
       <c r="G135" s="35"/>
@@ -8754,13 +8789,13 @@
     </row>
     <row r="136" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C136" s="34"/>
-      <c r="D136" s="10" t="s">
+      <c r="D136" s="46" t="s">
         <v>412</v>
       </c>
-      <c r="E136" s="10">
+      <c r="E136" s="46">
         <v>7</v>
       </c>
-      <c r="F136" s="16">
+      <c r="F136" s="47">
         <v>23</v>
       </c>
       <c r="G136" s="35"/>
@@ -8771,13 +8806,13 @@
     </row>
     <row r="137" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C137" s="34"/>
-      <c r="D137" s="10" t="s">
+      <c r="D137" s="46" t="s">
         <v>413</v>
       </c>
-      <c r="E137" s="10">
+      <c r="E137" s="46">
         <v>6</v>
       </c>
-      <c r="F137" s="16">
+      <c r="F137" s="47">
         <v>8</v>
       </c>
       <c r="G137" s="35"/>
@@ -8788,13 +8823,13 @@
     </row>
     <row r="138" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C138" s="34"/>
-      <c r="D138" s="10" t="s">
+      <c r="D138" s="46" t="s">
         <v>414</v>
       </c>
-      <c r="E138" s="10">
+      <c r="E138" s="46">
         <v>2</v>
       </c>
-      <c r="F138" s="16">
+      <c r="F138" s="47">
         <v>49</v>
       </c>
       <c r="G138" s="35"/>
@@ -8805,13 +8840,13 @@
     </row>
     <row r="139" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C139" s="34"/>
-      <c r="D139" s="10" t="s">
+      <c r="D139" s="46" t="s">
         <v>415</v>
       </c>
-      <c r="E139" s="10">
+      <c r="E139" s="46">
         <v>2</v>
       </c>
-      <c r="F139" s="16">
+      <c r="F139" s="47">
         <v>41</v>
       </c>
       <c r="G139" s="35"/>
@@ -8822,13 +8857,13 @@
     </row>
     <row r="140" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C140" s="34"/>
-      <c r="D140" s="10" t="s">
+      <c r="D140" s="46" t="s">
         <v>416</v>
       </c>
-      <c r="E140" s="10">
+      <c r="E140" s="46">
         <v>5</v>
       </c>
-      <c r="F140" s="16">
+      <c r="F140" s="47">
         <v>25</v>
       </c>
       <c r="G140" s="24" t="s">
@@ -8847,28 +8882,28 @@
     </row>
     <row r="141" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C141" s="34"/>
-      <c r="D141" s="11" t="s">
+      <c r="D141" s="48" t="s">
         <v>417</v>
       </c>
-      <c r="E141" s="11">
+      <c r="E141" s="48">
         <v>7</v>
       </c>
-      <c r="F141" s="17">
+      <c r="F141" s="49">
         <v>6</v>
       </c>
-      <c r="G141" s="7">
+      <c r="G141" s="57">
         <f>SUM(E135:E141)</f>
         <v>30</v>
       </c>
-      <c r="H141" s="2">
+      <c r="H141" s="58">
         <f>SUM(F135:F141)</f>
         <v>201</v>
       </c>
-      <c r="I141" s="6">
+      <c r="I141" s="59">
         <f>G141+(H141/60)</f>
         <v>33.35</v>
       </c>
-      <c r="J141" s="5">
+      <c r="J141" s="56">
         <v>1</v>
       </c>
       <c r="K141" s="37"/>

</xml_diff>